<commit_message>
made a loop to run over number of beads. domain and beam are set relative to the radius of gyration
</commit_message>
<xml_diff>
--- a/Documents/histoneSignalLossAndRecovery.xlsx
+++ b/Documents/histoneSignalLossAndRecovery.xlsx
@@ -54,12 +54,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -77,16 +76,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -215,245 +205,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>recovery/loss</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ee4000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$R$82:$R$98</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.159090909090909</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.294736842105263</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.536931818181818</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.777777777777778</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.13513513513513</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.42028985507246</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.64230769230769</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.86666666666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.23275862068966</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.45</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.72222222222222</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.74509803921569</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.0625</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.30978260869565</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.42045454545455</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="58970972"/>
-        <c:axId val="78097809"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="58970972"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="900">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>time post UVC [min]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="78097809"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="78097809"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="900">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>recovery/loss</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="58970972"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -644,11 +396,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="69426663"/>
-        <c:axId val="20573995"/>
+        <c:axId val="83571189"/>
+        <c:axId val="42879981"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69426663"/>
+        <c:axId val="83571189"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,14 +416,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20573995"/>
+        <c:crossAx val="42879981"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20573995"/>
+        <c:axId val="42879981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +448,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69426663"/>
+        <c:crossAx val="83571189"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -731,30 +483,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Loss-Recovery</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -783,6 +515,66 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$82:$L$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$M$82:$M$98</c:f>
@@ -845,11 +637,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47075380"/>
-        <c:axId val="63112149"/>
+        <c:axId val="68647421"/>
+        <c:axId val="94756234"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47075380"/>
+        <c:axId val="68647421"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,10 +657,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>time Post UVC</a:t>
+                  <a:t>time Post  UVC [min]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -885,11 +677,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="63112149"/>
+        <c:crossAx val="94756234"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63112149"/>
+        <c:axId val="94756234"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,10 +706,11 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Difference in histone signal loss %</a:t>
+                  <a:t>%loss-%recovery
+</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -934,7 +727,285 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47075380"/>
+        <c:crossAx val="68647421"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$82:$Q$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$82:$R$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.159090909090909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.294736842105263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.536931818181818</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.13513513513513</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.42028985507246</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.64230769230769</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.86666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.23275862068966</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.72222222222222</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.74509803921569</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.30978260869565</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.42045454545455</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="45741811"/>
+        <c:axId val="83728454"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="45741811"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>time post UVC [min]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="83728454"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="83728454"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>recovery/loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="45741811"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -974,15 +1045,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>739440</xdr:colOff>
+      <xdr:colOff>766440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>498960</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -990,8 +1061,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3579120" y="1023840"/>
-        <a:ext cx="7887240" cy="4092480"/>
+        <a:off x="3606120" y="1014840"/>
+        <a:ext cx="7887600" cy="4092480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1003,16 +1074,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>528840</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>782280</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>295200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:colOff>231120</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1025,8 +1096,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11496240" y="1042920"/>
-          <a:ext cx="4643280" cy="3046680"/>
+          <a:off x="10937160" y="4417920"/>
+          <a:ext cx="5138280" cy="2894400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1040,16 +1111,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>632520</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>699840</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>682920</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>750240</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1062,8 +1133,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9161640" y="6617160"/>
-          <a:ext cx="5740200" cy="2784240"/>
+          <a:off x="10854720" y="1588320"/>
+          <a:ext cx="5739840" cy="2783880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1077,16 +1148,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>361800</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>471600</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>198360</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1094,8 +1165,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5639760" y="15873840"/>
-        <a:ext cx="5759640" cy="3241440"/>
+        <a:off x="471600" y="16506360"/>
+        <a:ext cx="8255880" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1107,16 +1178,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>652680</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>620280</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>689040</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1124,8 +1195,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11620080" y="16227360"/>
-        <a:ext cx="5759640" cy="3241800"/>
+        <a:off x="9149400" y="16371720"/>
+        <a:ext cx="5758560" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1145,8 +1216,8 @@
   </sheetPr>
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U91" activeCellId="0" sqref="U91"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1161,10 +1232,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -1173,6 +1260,14 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1181,6 +1276,14 @@
       <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1190,6 +1293,14 @@
         <f aca="false">6.4/10.5</f>
         <v>0.60952380952381</v>
       </c>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1199,6 +1310,14 @@
         <f aca="false">5.5/10.5</f>
         <v>0.523809523809524</v>
       </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1208,6 +1327,14 @@
         <f aca="false">4.75/10.5</f>
         <v>0.452380952380952</v>
       </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1217,6 +1344,14 @@
         <f aca="false">4.4/10.5</f>
         <v>0.419047619047619</v>
       </c>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1226,6 +1361,14 @@
         <f aca="false">4.05/10.5</f>
         <v>0.385714285714286</v>
       </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1235,6 +1378,14 @@
         <f aca="false">3.7/10.5</f>
         <v>0.352380952380952</v>
       </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1244,6 +1395,14 @@
         <f aca="false">3.45/10.5</f>
         <v>0.328571428571429</v>
       </c>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1253,6 +1412,14 @@
         <f aca="false">3.25/10.5</f>
         <v>0.30952380952381</v>
       </c>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1262,6 +1429,14 @@
         <f aca="false">3/10.5</f>
         <v>0.285714285714286</v>
       </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1271,6 +1446,14 @@
         <f aca="false">2.9/10.5</f>
         <v>0.276190476190476</v>
       </c>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1280,6 +1463,14 @@
         <f aca="false">2.75/10.5</f>
         <v>0.261904761904762</v>
       </c>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="Q15" s="0"/>
+      <c r="R15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1289,6 +1480,14 @@
         <f aca="false">2.7/10.5</f>
         <v>0.257142857142857</v>
       </c>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="K16" s="0"/>
+      <c r="L16" s="0"/>
+      <c r="M16" s="0"/>
+      <c r="Q16" s="0"/>
+      <c r="R16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1298,6 +1497,14 @@
         <f aca="false">2.5/10.5</f>
         <v>0.238095238095238</v>
       </c>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+      <c r="M17" s="0"/>
+      <c r="Q17" s="0"/>
+      <c r="R17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1307,6 +1514,14 @@
         <f aca="false">2.55/10.5</f>
         <v>0.242857142857143</v>
       </c>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="Q18" s="0"/>
+      <c r="R18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1316,6 +1531,14 @@
         <f aca="false">2.4/10.5</f>
         <v>0.228571428571429</v>
       </c>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="Q19" s="0"/>
+      <c r="R19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1325,6 +1548,14 @@
         <f aca="false">2.3/10.5</f>
         <v>0.219047619047619</v>
       </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
+      <c r="Q20" s="0"/>
+      <c r="R20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1334,6 +1565,14 @@
         <f aca="false">2.2/10.5</f>
         <v>0.20952380952381</v>
       </c>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="Q21" s="0"/>
+      <c r="R21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1343,6 +1582,14 @@
         <f aca="false">2.1/10.5</f>
         <v>0.2</v>
       </c>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
+      <c r="Q22" s="0"/>
+      <c r="R22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1352,6 +1599,14 @@
         <f aca="false">2.01/10.5</f>
         <v>0.191428571428571</v>
       </c>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="I23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="Q23" s="0"/>
+      <c r="R23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1361,53 +1616,208 @@
         <f aca="false">2/10.5</f>
         <v>0.19047619047619</v>
       </c>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="I24" s="0"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
+      <c r="Q24" s="0"/>
+      <c r="R24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="Q25" s="0"/>
+      <c r="R25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="Q26" s="0"/>
+      <c r="R26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="Q27" s="0"/>
+      <c r="R27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="Q28" s="0"/>
+      <c r="R28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="Q29" s="0"/>
+      <c r="R29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
+      <c r="Q30" s="0"/>
+      <c r="R30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+      <c r="Q31" s="0"/>
+      <c r="R31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+      <c r="Q32" s="0"/>
+      <c r="R32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+      <c r="Q33" s="0"/>
+      <c r="R33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="Q34" s="0"/>
+      <c r="R34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="Q35" s="0"/>
+      <c r="R35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+      <c r="M36" s="0"/>
+      <c r="Q36" s="0"/>
+      <c r="R36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="I37" s="0"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
+      <c r="M37" s="0"/>
+      <c r="Q37" s="0"/>
+      <c r="R37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
+      <c r="Q38" s="0"/>
+      <c r="R38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="Q39" s="0"/>
+      <c r="R39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
+      <c r="Q40" s="0"/>
+      <c r="R40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -1416,6 +1826,14 @@
       <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0"/>
+      <c r="Q41" s="0"/>
+      <c r="R41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1424,6 +1842,14 @@
       <c r="B42" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0"/>
+      <c r="Q42" s="0"/>
+      <c r="R42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -1433,6 +1859,14 @@
         <f aca="false">0.5/6</f>
         <v>0.0833333333333333</v>
       </c>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
+      <c r="Q43" s="0"/>
+      <c r="R43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -1442,6 +1876,14 @@
         <f aca="false">0.5/6</f>
         <v>0.0833333333333333</v>
       </c>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
+      <c r="Q44" s="0"/>
+      <c r="R44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -1451,6 +1893,14 @@
         <f aca="false">0.7/6</f>
         <v>0.116666666666667</v>
       </c>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="Q45" s="0"/>
+      <c r="R45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -1460,6 +1910,14 @@
         <f aca="false">0.8/6</f>
         <v>0.133333333333333</v>
       </c>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="Q46" s="0"/>
+      <c r="R46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -1469,6 +1927,14 @@
         <f aca="false">1.15/6</f>
         <v>0.191666666666667</v>
       </c>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+      <c r="Q47" s="0"/>
+      <c r="R47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -1478,6 +1944,14 @@
         <f aca="false">1.35/6</f>
         <v>0.225</v>
       </c>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
+      <c r="I48" s="0"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
+      <c r="Q48" s="0"/>
+      <c r="R48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -1487,6 +1961,14 @@
         <f aca="false">1.4/6</f>
         <v>0.233333333333333</v>
       </c>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
+      <c r="I49" s="0"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
+      <c r="M49" s="0"/>
+      <c r="Q49" s="0"/>
+      <c r="R49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -1496,6 +1978,14 @@
         <f aca="false">1.8/6</f>
         <v>0.3</v>
       </c>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="I50" s="0"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
+      <c r="Q50" s="0"/>
+      <c r="R50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -1505,6 +1995,14 @@
         <f aca="false">2.3/6</f>
         <v>0.383333333333333</v>
       </c>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
+      <c r="I51" s="0"/>
+      <c r="K51" s="0"/>
+      <c r="L51" s="0"/>
+      <c r="M51" s="0"/>
+      <c r="Q51" s="0"/>
+      <c r="R51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -1514,6 +2012,14 @@
         <f aca="false">2.4/6</f>
         <v>0.4</v>
       </c>
+      <c r="E52" s="0"/>
+      <c r="F52" s="0"/>
+      <c r="I52" s="0"/>
+      <c r="K52" s="0"/>
+      <c r="L52" s="0"/>
+      <c r="M52" s="0"/>
+      <c r="Q52" s="0"/>
+      <c r="R52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -1523,6 +2029,14 @@
         <f aca="false">2.55/6</f>
         <v>0.425</v>
       </c>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
+      <c r="I53" s="0"/>
+      <c r="K53" s="0"/>
+      <c r="L53" s="0"/>
+      <c r="M53" s="0"/>
+      <c r="Q53" s="0"/>
+      <c r="R53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -1532,6 +2046,14 @@
         <f aca="false">2.8/6</f>
         <v>0.466666666666667</v>
       </c>
+      <c r="E54" s="0"/>
+      <c r="F54" s="0"/>
+      <c r="I54" s="0"/>
+      <c r="K54" s="0"/>
+      <c r="L54" s="0"/>
+      <c r="M54" s="0"/>
+      <c r="Q54" s="0"/>
+      <c r="R54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -1541,6 +2063,14 @@
         <f aca="false">2.85/6</f>
         <v>0.475</v>
       </c>
+      <c r="E55" s="0"/>
+      <c r="F55" s="0"/>
+      <c r="I55" s="0"/>
+      <c r="K55" s="0"/>
+      <c r="L55" s="0"/>
+      <c r="M55" s="0"/>
+      <c r="Q55" s="0"/>
+      <c r="R55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -1550,6 +2080,14 @@
         <f aca="false">3.05/6</f>
         <v>0.508333333333333</v>
       </c>
+      <c r="E56" s="0"/>
+      <c r="F56" s="0"/>
+      <c r="I56" s="0"/>
+      <c r="K56" s="0"/>
+      <c r="L56" s="0"/>
+      <c r="M56" s="0"/>
+      <c r="Q56" s="0"/>
+      <c r="R56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -1559,6 +2097,14 @@
         <f aca="false">3.2/6</f>
         <v>0.533333333333333</v>
       </c>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="I57" s="0"/>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="Q57" s="0"/>
+      <c r="R57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -1568,6 +2114,14 @@
         <f aca="false">3.2/6</f>
         <v>0.533333333333333</v>
       </c>
+      <c r="E58" s="0"/>
+      <c r="F58" s="0"/>
+      <c r="I58" s="0"/>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+      <c r="M58" s="0"/>
+      <c r="Q58" s="0"/>
+      <c r="R58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -1577,6 +2131,14 @@
         <f aca="false">3.6/6</f>
         <v>0.6</v>
       </c>
+      <c r="E59" s="0"/>
+      <c r="F59" s="0"/>
+      <c r="I59" s="0"/>
+      <c r="K59" s="0"/>
+      <c r="L59" s="0"/>
+      <c r="M59" s="0"/>
+      <c r="Q59" s="0"/>
+      <c r="R59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
@@ -1586,6 +2148,14 @@
         <f aca="false">3.7/6</f>
         <v>0.616666666666667</v>
       </c>
+      <c r="E60" s="0"/>
+      <c r="F60" s="0"/>
+      <c r="I60" s="0"/>
+      <c r="K60" s="0"/>
+      <c r="L60" s="0"/>
+      <c r="M60" s="0"/>
+      <c r="Q60" s="0"/>
+      <c r="R60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -1595,6 +2165,14 @@
         <f aca="false">3.75/6</f>
         <v>0.625</v>
       </c>
+      <c r="E61" s="0"/>
+      <c r="F61" s="0"/>
+      <c r="I61" s="0"/>
+      <c r="K61" s="0"/>
+      <c r="L61" s="0"/>
+      <c r="M61" s="0"/>
+      <c r="Q61" s="0"/>
+      <c r="R61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -1604,6 +2182,14 @@
         <f aca="false">3.85/6</f>
         <v>0.641666666666667</v>
       </c>
+      <c r="E62" s="0"/>
+      <c r="F62" s="0"/>
+      <c r="I62" s="0"/>
+      <c r="K62" s="0"/>
+      <c r="L62" s="0"/>
+      <c r="M62" s="0"/>
+      <c r="Q62" s="0"/>
+      <c r="R62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -1613,6 +2199,14 @@
         <f aca="false">3.8/6</f>
         <v>0.633333333333333</v>
       </c>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
+      <c r="I63" s="0"/>
+      <c r="K63" s="0"/>
+      <c r="L63" s="0"/>
+      <c r="M63" s="0"/>
+      <c r="Q63" s="0"/>
+      <c r="R63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -1622,6 +2216,14 @@
         <f aca="false">4.2/6</f>
         <v>0.7</v>
       </c>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+      <c r="I64" s="0"/>
+      <c r="K64" s="0"/>
+      <c r="L64" s="0"/>
+      <c r="M64" s="0"/>
+      <c r="Q64" s="0"/>
+      <c r="R64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -1631,6 +2233,14 @@
         <f aca="false">4.15/6</f>
         <v>0.691666666666667</v>
       </c>
+      <c r="E65" s="0"/>
+      <c r="F65" s="0"/>
+      <c r="I65" s="0"/>
+      <c r="K65" s="0"/>
+      <c r="L65" s="0"/>
+      <c r="M65" s="0"/>
+      <c r="Q65" s="0"/>
+      <c r="R65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -1640,6 +2250,14 @@
         <f aca="false">4.2/6</f>
         <v>0.7</v>
       </c>
+      <c r="E66" s="0"/>
+      <c r="F66" s="0"/>
+      <c r="I66" s="0"/>
+      <c r="K66" s="0"/>
+      <c r="L66" s="0"/>
+      <c r="M66" s="0"/>
+      <c r="Q66" s="0"/>
+      <c r="R66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -1649,6 +2267,14 @@
         <f aca="false">4.2/6</f>
         <v>0.7</v>
       </c>
+      <c r="E67" s="0"/>
+      <c r="F67" s="0"/>
+      <c r="I67" s="0"/>
+      <c r="K67" s="0"/>
+      <c r="L67" s="0"/>
+      <c r="M67" s="0"/>
+      <c r="Q67" s="0"/>
+      <c r="R67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -1658,6 +2284,14 @@
         <f aca="false">4/6</f>
         <v>0.666666666666667</v>
       </c>
+      <c r="E68" s="0"/>
+      <c r="F68" s="0"/>
+      <c r="I68" s="0"/>
+      <c r="K68" s="0"/>
+      <c r="L68" s="0"/>
+      <c r="M68" s="0"/>
+      <c r="Q68" s="0"/>
+      <c r="R68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -1667,6 +2301,14 @@
         <f aca="false">4.05/6</f>
         <v>0.675</v>
       </c>
+      <c r="E69" s="0"/>
+      <c r="F69" s="0"/>
+      <c r="I69" s="0"/>
+      <c r="K69" s="0"/>
+      <c r="L69" s="0"/>
+      <c r="M69" s="0"/>
+      <c r="Q69" s="0"/>
+      <c r="R69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -1676,6 +2318,14 @@
         <f aca="false">4.2/6</f>
         <v>0.7</v>
       </c>
+      <c r="E70" s="0"/>
+      <c r="F70" s="0"/>
+      <c r="I70" s="0"/>
+      <c r="K70" s="0"/>
+      <c r="L70" s="0"/>
+      <c r="M70" s="0"/>
+      <c r="Q70" s="0"/>
+      <c r="R70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -1685,6 +2335,14 @@
         <f aca="false">4.3/6</f>
         <v>0.716666666666667</v>
       </c>
+      <c r="E71" s="0"/>
+      <c r="F71" s="0"/>
+      <c r="I71" s="0"/>
+      <c r="K71" s="0"/>
+      <c r="L71" s="0"/>
+      <c r="M71" s="0"/>
+      <c r="Q71" s="0"/>
+      <c r="R71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
@@ -1694,6 +2352,14 @@
         <f aca="false">4.35/6</f>
         <v>0.725</v>
       </c>
+      <c r="E72" s="0"/>
+      <c r="F72" s="0"/>
+      <c r="I72" s="0"/>
+      <c r="K72" s="0"/>
+      <c r="L72" s="0"/>
+      <c r="M72" s="0"/>
+      <c r="Q72" s="0"/>
+      <c r="R72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -1703,6 +2369,14 @@
         <f aca="false">4.4/6</f>
         <v>0.733333333333333</v>
       </c>
+      <c r="E73" s="0"/>
+      <c r="F73" s="0"/>
+      <c r="I73" s="0"/>
+      <c r="K73" s="0"/>
+      <c r="L73" s="0"/>
+      <c r="M73" s="0"/>
+      <c r="Q73" s="0"/>
+      <c r="R73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
@@ -1712,19 +2386,80 @@
         <f aca="false">4.3/6</f>
         <v>0.716666666666667</v>
       </c>
+      <c r="E74" s="0"/>
+      <c r="F74" s="0"/>
+      <c r="I74" s="0"/>
+      <c r="K74" s="0"/>
+      <c r="L74" s="0"/>
+      <c r="M74" s="0"/>
+      <c r="Q74" s="0"/>
+      <c r="R74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0"/>
+      <c r="B75" s="0"/>
+      <c r="E75" s="0"/>
+      <c r="F75" s="0"/>
+      <c r="I75" s="0"/>
+      <c r="K75" s="0"/>
+      <c r="L75" s="0"/>
+      <c r="M75" s="0"/>
+      <c r="Q75" s="0"/>
+      <c r="R75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0"/>
+      <c r="B76" s="0"/>
+      <c r="E76" s="0"/>
+      <c r="F76" s="0"/>
+      <c r="I76" s="0"/>
+      <c r="K76" s="0"/>
+      <c r="L76" s="0"/>
+      <c r="M76" s="0"/>
+      <c r="Q76" s="0"/>
+      <c r="R76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B77" s="0"/>
+      <c r="E77" s="0"/>
+      <c r="F77" s="0"/>
+      <c r="I77" s="0"/>
+      <c r="K77" s="0"/>
+      <c r="L77" s="0"/>
+      <c r="M77" s="0"/>
+      <c r="Q77" s="0"/>
+      <c r="R77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="E78" s="0"/>
+      <c r="F78" s="0"/>
+      <c r="I78" s="0"/>
+      <c r="K78" s="0"/>
+      <c r="L78" s="0"/>
+      <c r="M78" s="0"/>
+      <c r="Q78" s="0"/>
+      <c r="R78" s="0"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B79" s="0"/>
       <c r="E79" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F79" s="0"/>
+      <c r="I79" s="0"/>
+      <c r="K79" s="0"/>
+      <c r="L79" s="0"/>
+      <c r="M79" s="0"/>
+      <c r="Q79" s="0"/>
+      <c r="R79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
@@ -1739,6 +2474,12 @@
       <c r="F80" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I80" s="0"/>
+      <c r="K80" s="0"/>
+      <c r="L80" s="0"/>
+      <c r="M80" s="0"/>
+      <c r="Q80" s="0"/>
+      <c r="R80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">

</xml_diff>